<commit_message>
keine geschwindigkeit in csv
</commit_message>
<xml_diff>
--- a/angabe1/data/2017/Messungen_2017_Geschwindigkeit_Ebene.xlsx
+++ b/angabe1/data/2017/Messungen_2017_Geschwindigkeit_Ebene.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Runde</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>getrödelt</t>
-  </si>
-  <si>
-    <t>Geschwindigkeit</t>
   </si>
   <si>
     <t>ID_Proband</t>
@@ -43,9 +40,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -75,7 +69,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -85,7 +79,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -374,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E67"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,28 +379,24 @@
     <col min="2" max="2" width="13.7109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="15" style="2" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -417,12 +406,8 @@
       <c r="C2" s="4">
         <v>17.649999999999999</v>
       </c>
-      <c r="E2" s="5">
-        <f>27.3/C2</f>
-        <v>1.5467422096317283</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -432,12 +417,8 @@
       <c r="C3" s="4">
         <v>17.37</v>
       </c>
-      <c r="E3" s="5">
-        <f t="shared" ref="E3:E66" si="0">27.3/C3</f>
-        <v>1.5716753022452503</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -447,12 +428,8 @@
       <c r="C4" s="4">
         <v>17.88</v>
       </c>
-      <c r="E4" s="5">
-        <f t="shared" si="0"/>
-        <v>1.5268456375838928</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -462,12 +439,8 @@
       <c r="C5" s="4">
         <v>15.81</v>
       </c>
-      <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7267552182163188</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1</v>
       </c>
@@ -477,12 +450,8 @@
       <c r="C6" s="4">
         <v>15.97</v>
       </c>
-      <c r="E6" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7094552285535378</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
@@ -492,12 +461,8 @@
       <c r="C7" s="4">
         <v>18.84</v>
       </c>
-      <c r="E7" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4490445859872612</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -510,12 +475,8 @@
       <c r="D8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1947483588621444</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1</v>
       </c>
@@ -525,12 +486,8 @@
       <c r="C9" s="4">
         <v>17.47</v>
       </c>
-      <c r="E9" s="5">
-        <f t="shared" si="0"/>
-        <v>1.5626788780767031</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>1</v>
       </c>
@@ -540,12 +497,8 @@
       <c r="C10" s="4">
         <v>18.760000000000002</v>
       </c>
-      <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4552238805970148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>1</v>
       </c>
@@ -555,12 +508,8 @@
       <c r="C11" s="4">
         <v>22.08</v>
       </c>
-      <c r="E11" s="5">
-        <f t="shared" si="0"/>
-        <v>1.236413043478261</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -570,12 +519,8 @@
       <c r="C12" s="4">
         <v>18.25</v>
       </c>
-      <c r="E12" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4958904109589042</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -585,12 +530,8 @@
       <c r="C13" s="4">
         <v>17.5</v>
       </c>
-      <c r="E13" s="5">
-        <f t="shared" si="0"/>
-        <v>1.56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>1</v>
       </c>
@@ -601,140 +542,104 @@
       <c r="C14" s="4">
         <v>21.25</v>
       </c>
-      <c r="E14" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2847058823529411</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>1</v>
       </c>
       <c r="B15" s="2">
-        <f t="shared" ref="B15:B22" si="1">B14+1</f>
+        <f t="shared" ref="B15:B22" si="0">B14+1</f>
         <v>14</v>
       </c>
       <c r="C15" s="4">
         <v>16.32</v>
       </c>
-      <c r="E15" s="5">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2">
         <f t="shared" si="0"/>
-        <v>1.6727941176470589</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2">
-        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C16" s="4">
         <v>18.239999999999998</v>
       </c>
-      <c r="E16" s="5">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2">
         <f t="shared" si="0"/>
-        <v>1.4967105263157896</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2">
-        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C17" s="4">
         <v>19.71</v>
       </c>
-      <c r="E17" s="5">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2">
         <f t="shared" si="0"/>
-        <v>1.3850837138508372</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2">
-        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C18" s="4">
         <v>19.82</v>
       </c>
-      <c r="E18" s="5">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
         <f t="shared" si="0"/>
-        <v>1.3773965691220988</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2">
-        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C19" s="4">
         <v>16.25</v>
       </c>
-      <c r="E19" s="5">
-        <f>27.3/C19</f>
-        <v>1.68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>1</v>
       </c>
       <c r="B20" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C20" s="4">
         <v>19.809999999999999</v>
       </c>
-      <c r="E20" s="5">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2">
         <f t="shared" si="0"/>
-        <v>1.3780918727915195</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
-        <v>1</v>
-      </c>
-      <c r="B21" s="2">
-        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C21" s="4">
         <v>18.96</v>
       </c>
-      <c r="E21" s="5">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2">
         <f t="shared" si="0"/>
-        <v>1.4398734177215189</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
-        <v>1</v>
-      </c>
-      <c r="B22" s="2">
-        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C22" s="4">
         <v>17</v>
       </c>
-      <c r="E22" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6058823529411765</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>1</v>
       </c>
@@ -745,12 +650,8 @@
       <c r="C23" s="4">
         <v>19</v>
       </c>
-      <c r="E23" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4368421052631579</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>2</v>
       </c>
@@ -760,12 +661,8 @@
       <c r="C24" s="4">
         <v>17.53</v>
       </c>
-      <c r="E24" s="5">
-        <f t="shared" si="0"/>
-        <v>1.5573302909298345</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>2</v>
       </c>
@@ -775,12 +672,8 @@
       <c r="C25" s="4">
         <v>16.34</v>
       </c>
-      <c r="E25" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6707466340269279</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>2</v>
       </c>
@@ -790,12 +683,8 @@
       <c r="C26" s="4">
         <v>16.899999999999999</v>
       </c>
-      <c r="E26" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6153846153846156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>2</v>
       </c>
@@ -805,12 +694,8 @@
       <c r="C27" s="4">
         <v>15.62</v>
       </c>
-      <c r="E27" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7477592829705506</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>2</v>
       </c>
@@ -820,12 +705,8 @@
       <c r="C28" s="4">
         <v>16.149999999999999</v>
       </c>
-      <c r="E28" s="5">
-        <f t="shared" si="0"/>
-        <v>1.690402476780186</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>2</v>
       </c>
@@ -835,12 +716,8 @@
       <c r="C29" s="4">
         <v>19</v>
       </c>
-      <c r="E29" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4368421052631579</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>2</v>
       </c>
@@ -853,12 +730,8 @@
       <c r="D30" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E30" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1885067479320854</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>2</v>
       </c>
@@ -868,12 +741,8 @@
       <c r="C31" s="4">
         <v>18.29</v>
       </c>
-      <c r="E31" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4926189174412248</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>2</v>
       </c>
@@ -883,12 +752,8 @@
       <c r="C32" s="4">
         <v>21.13</v>
       </c>
-      <c r="E32" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2920018930430668</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>2</v>
       </c>
@@ -898,12 +763,8 @@
       <c r="C33" s="4">
         <v>22.45</v>
       </c>
-      <c r="E33" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2160356347438754</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>2</v>
       </c>
@@ -913,12 +774,8 @@
       <c r="C34" s="4">
         <v>18.66</v>
       </c>
-      <c r="E34" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4630225080385852</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>2</v>
       </c>
@@ -928,12 +785,8 @@
       <c r="C35" s="4">
         <v>18.34</v>
       </c>
-      <c r="E35" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4885496183206108</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>2</v>
       </c>
@@ -944,156 +797,116 @@
       <c r="C36" s="4">
         <v>20.32</v>
       </c>
-      <c r="E36" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3435039370078741</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>2</v>
       </c>
       <c r="B37" s="2">
-        <f t="shared" ref="B37:B45" si="2">B36+1</f>
+        <f t="shared" ref="B37:B45" si="1">B36+1</f>
         <v>14</v>
       </c>
       <c r="C37" s="4">
         <v>16.66</v>
       </c>
-      <c r="E37" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6386554621848739</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>2</v>
       </c>
       <c r="B38" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="C38" s="4">
         <v>18.59</v>
       </c>
-      <c r="E38" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4685314685314685</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>2</v>
       </c>
       <c r="B39" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="C39" s="4">
         <v>20.03</v>
       </c>
-      <c r="E39" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3629555666500248</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>2</v>
       </c>
       <c r="B40" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="C40" s="4">
         <v>19.559999999999999</v>
       </c>
-      <c r="E40" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3957055214723928</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>2</v>
       </c>
       <c r="B41" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="C41" s="4">
         <v>16.690000000000001</v>
       </c>
-      <c r="E41" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6357100059916116</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>2</v>
       </c>
       <c r="B42" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="C42" s="4">
         <v>18.91</v>
       </c>
-      <c r="E42" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4436805922792173</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>2</v>
       </c>
       <c r="B43" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C43" s="4">
         <v>19.59</v>
       </c>
-      <c r="E43" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3935681470137826</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>2</v>
       </c>
       <c r="B44" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="C44" s="4">
         <v>16.97</v>
       </c>
-      <c r="E44" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6087212728344138</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>2</v>
       </c>
       <c r="B45" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="C45" s="4">
         <v>18.72</v>
       </c>
-      <c r="E45" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4583333333333335</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>3</v>
       </c>
@@ -1103,12 +916,8 @@
       <c r="C46" s="4">
         <v>17</v>
       </c>
-      <c r="E46" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6058823529411765</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>3</v>
       </c>
@@ -1118,12 +927,8 @@
       <c r="C47" s="4">
         <v>16.72</v>
       </c>
-      <c r="E47" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6327751196172251</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>3</v>
       </c>
@@ -1133,12 +938,8 @@
       <c r="C48" s="4">
         <v>17.09</v>
       </c>
-      <c r="E48" s="5">
-        <f t="shared" si="0"/>
-        <v>1.5974253949678174</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>3</v>
       </c>
@@ -1148,12 +949,8 @@
       <c r="C49" s="4">
         <v>16.62</v>
       </c>
-      <c r="E49" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6425992779783394</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>3</v>
       </c>
@@ -1163,12 +960,8 @@
       <c r="C50" s="4">
         <v>16.940000000000001</v>
       </c>
-      <c r="E50" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6115702479338843</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>3</v>
       </c>
@@ -1178,12 +971,8 @@
       <c r="C51" s="4">
         <v>18.47</v>
       </c>
-      <c r="E51" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4780725500812129</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>3</v>
       </c>
@@ -1196,12 +985,8 @@
       <c r="D52" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E52" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1460957178841309</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>3</v>
       </c>
@@ -1211,12 +996,8 @@
       <c r="C53" s="4">
         <v>18.95</v>
       </c>
-      <c r="E53" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4406332453825859</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>3</v>
       </c>
@@ -1226,12 +1007,8 @@
       <c r="C54" s="4">
         <v>19.649999999999999</v>
       </c>
-      <c r="E54" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3893129770992367</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>3</v>
       </c>
@@ -1241,12 +1018,8 @@
       <c r="C55" s="4">
         <v>22.5</v>
       </c>
-      <c r="E55" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2133333333333334</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>3</v>
       </c>
@@ -1256,12 +1029,8 @@
       <c r="C56" s="4">
         <v>19.850000000000001</v>
       </c>
-      <c r="E56" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3753148614609572</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>3</v>
       </c>
@@ -1271,12 +1040,8 @@
       <c r="C57" s="4">
         <v>18.13</v>
       </c>
-      <c r="E57" s="5">
-        <f t="shared" si="0"/>
-        <v>1.5057915057915059</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>3</v>
       </c>
@@ -1287,153 +1052,113 @@
       <c r="C58" s="4">
         <v>19.309999999999999</v>
       </c>
-      <c r="E58" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4137752459865356</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>3</v>
       </c>
       <c r="B59" s="2">
-        <f t="shared" ref="B59:B67" si="3">B58+1</f>
+        <f t="shared" ref="B59:B67" si="2">B58+1</f>
         <v>14</v>
       </c>
       <c r="C59" s="4">
         <v>17.41</v>
       </c>
-      <c r="E59" s="5">
-        <f t="shared" si="0"/>
-        <v>1.5680643308443423</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>3</v>
       </c>
       <c r="B60" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="C60" s="4">
         <v>19.54</v>
       </c>
-      <c r="E60" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3971340839303992</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>3</v>
       </c>
       <c r="B61" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C61" s="4">
         <v>20.18</v>
       </c>
-      <c r="E61" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3528245787908821</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>3</v>
       </c>
       <c r="B62" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="C62" s="4">
         <v>18.71</v>
       </c>
-      <c r="E62" s="5">
-        <f t="shared" si="0"/>
-        <v>1.459112773917691</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>3</v>
       </c>
       <c r="B63" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="C63" s="4">
         <v>16.940000000000001</v>
       </c>
-      <c r="E63" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6115702479338843</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>3</v>
       </c>
       <c r="B64" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="C64" s="4">
         <v>18.25</v>
       </c>
-      <c r="E64" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4958904109589042</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>3</v>
       </c>
       <c r="B65" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="C65" s="4">
         <v>20</v>
       </c>
-      <c r="E65" s="5">
-        <f t="shared" si="0"/>
-        <v>1.365</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>3</v>
       </c>
       <c r="B66" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="C66" s="4">
         <v>16.37</v>
       </c>
-      <c r="E66" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6676847892486255</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>3</v>
       </c>
       <c r="B67" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="C67" s="4">
         <v>20.09</v>
-      </c>
-      <c r="E67" s="5">
-        <f t="shared" ref="E67" si="4">27.3/C67</f>
-        <v>1.3588850174216027</v>
       </c>
     </row>
   </sheetData>

</xml_diff>